<commit_message>
push code 23-6-2024 3:06
</commit_message>
<xml_diff>
--- a/Source/OMT/Equipment/Datasheet/Địa chỉ IO các thiết bị ở các trạm để làm lại datasheet.xlsx
+++ b/Source/OMT/Equipment/Datasheet/Địa chỉ IO các thiết bị ở các trạm để làm lại datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wembley_Medical_AR\Source\OMT\Equipment\Datasheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5B76EC-E7E4-49CB-970F-4926B4D9E85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394DAED0-C124-4939-B636-2230789DCF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F05BE189-F7B8-4A8D-8EFD-E1055AC6C6F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>MÃ THIẾT BỊ</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>ĐỊA CHỈ I/O, Chức năng thiết bị</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X14, X15, X16,X17,X20:   S1 Chem Spray Tray Pos Chk 1-5
+ X13:  S1 Drying-2 Chk Pos Snr
+ X21:  S1 Drying-1 Chk Pos Snr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Y16: Drying Sys 1 Cyl Up
+ Y17: Drying 1 Cyl Dn</t>
   </si>
 </sst>
 </file>
@@ -228,32 +237,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,395 +603,278 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA6B740-6190-4C63-9928-73FA84180CAC}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="B1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.796875" style="1"/>
-    <col min="2" max="2" width="28.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="32.19921875" style="1" customWidth="1"/>
-    <col min="4" max="6" width="20.69921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="49" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.59765625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="20.69921875" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="8"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
+      <c r="C14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="2:5" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+      <c r="C25" s="6"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="2:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="2:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="8" t="s">
+      <c r="C27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
+      <c r="C28" s="6"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
+      <c r="C29" s="6"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-    </row>
+      <c r="C30" s="6"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:E1"/>

</xml_diff>